<commit_message>
various changes, BOM additions
</commit_message>
<xml_diff>
--- a/documentation/BOM.xlsx
+++ b/documentation/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncross\Documents\siweed\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E289A50B-CAC9-4EAB-B51F-546B05C21D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A509D2-CBFB-4740-94E6-E7093251C67A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1995" windowWidth="29040" windowHeight="17640" xr2:uid="{A070BE1D-938F-4FAE-920C-E8C343EADAC0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{A070BE1D-938F-4FAE-920C-E8C343EADAC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
   <si>
     <t>Designator</t>
   </si>
@@ -186,14 +186,112 @@
   </si>
   <si>
     <t>Electronics Only Cost:</t>
+  </si>
+  <si>
+    <t>Electronics:</t>
+  </si>
+  <si>
+    <t>Other:</t>
+  </si>
+  <si>
+    <t>Decorations:</t>
+  </si>
+  <si>
+    <t>Lighthouse</t>
+  </si>
+  <si>
+    <t>https://factorydirecthobbies.com/products/preorder-walthers-cornerstone-933-3656-eagle-point-lighthouse-kit-8-1-8-x-3-x-8-7-8-20-3-x-7-5-x-22-8cm-ho?variant=39291075657791&amp;currency=USD&amp;utm_medium=product_sync&amp;utm_source=google&amp;utm_content=sag_organic&amp;utm_campaign=sag_organic&amp;utm_campaign=gs-2020-09-16&amp;utm_source=google&amp;utm_medium=smart_campaign&amp;gclid=EAIaIQobChMI2_Lt9Yne8QIVvGxvBB27rQC5EAQYAiABEgK43fD_BwE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Store Set </t>
+  </si>
+  <si>
+    <t>https://www.modeltrainstuff.com/motrak-models-ho-83006-applewood-general-store-with-freight-depot-kit/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House (1 story) </t>
+  </si>
+  <si>
+    <t>https://www.modeltrainstuff.com/Bachmann-HO-45432-Contemporary-House-Snap-Kit/</t>
+  </si>
+  <si>
+    <t>Fishing Shack</t>
+  </si>
+  <si>
+    <t>https://barmillsmodels.com/product/fishing-shack-ho/</t>
+  </si>
+  <si>
+    <t>Shed</t>
+  </si>
+  <si>
+    <t>https://www.mapleleaftrains.com/catalog/76231-garden-shed/</t>
+  </si>
+  <si>
+    <t>Street Lights</t>
+  </si>
+  <si>
+    <t>Seaweed (13 pack)</t>
+  </si>
+  <si>
+    <t>Grass Tufts (withered yellow)</t>
+  </si>
+  <si>
+    <t>Grass Tufts (green)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sand (38 lb) </t>
+  </si>
+  <si>
+    <t>Sandpaper (48 pack)</t>
+  </si>
+  <si>
+    <t>Grass Shaker</t>
+  </si>
+  <si>
+    <t>Palm trees</t>
+  </si>
+  <si>
+    <t>Gravel</t>
+  </si>
+  <si>
+    <t>Cliff Rocks</t>
+  </si>
+  <si>
+    <t>Double Sided Tape</t>
+  </si>
+  <si>
+    <t>Angle Brace</t>
+  </si>
+  <si>
+    <t>Angle Brace Screws</t>
+  </si>
+  <si>
+    <t>Styrofoam Sheets</t>
+  </si>
+  <si>
+    <t>Foam</t>
+  </si>
+  <si>
+    <t>Tweezers</t>
+  </si>
+  <si>
+    <t>Decorations Only Cost:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -221,8 +319,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,435 +636,876 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A88E862-9BB9-4130-9B0E-5C55249A1E9C}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.86328125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>34.950000000000003</v>
       </c>
-      <c r="E2">
-        <f>D2*C2</f>
+      <c r="E3">
+        <f>D3*C3</f>
         <v>34.950000000000003</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>37.4</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E23" si="0">D3*C3</f>
-        <v>74.8</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>37.4</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E50" si="0">D4*C4</f>
+        <v>74.8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>3.49</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>10.47</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
         <v>28.65</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>57.3</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
         <v>23.86</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>47.72</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>44</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>89.39</v>
-      </c>
-      <c r="E7">
-        <f t="shared" ref="E7" si="1">D7*C7</f>
-        <v>89.39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>87</v>
+        <v>89.39</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f t="shared" ref="E8" si="1">D8*C8</f>
+        <v>89.39</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>190.45</v>
+        <v>87</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>190.45</v>
+        <v>87</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>19.899999999999999</v>
+        <v>190.45</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>19.899999999999999</v>
+        <v>190.45</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>33.92</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>33.92</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="F11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>164.19</v>
+        <v>33.92</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>164.19</v>
+        <v>33.92</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>5.95</v>
+        <v>164.19</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>5.95</v>
+        <v>164.19</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>5.95</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>5.95</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
         <v>1075</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <f t="shared" si="0"/>
         <v>2150</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>37</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>122.65</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>122.65</v>
-      </c>
-      <c r="F15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
+        <v>122.65</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>122.65</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
         <v>8.9499999999999993</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <f t="shared" si="0"/>
         <v>8.9499999999999993</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>5</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <f t="shared" si="0"/>
         <v>5.6000000000000005</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>50.38</v>
+      </c>
+      <c r="E21">
+        <f>C21*D21</f>
+        <v>100.76</v>
+      </c>
+      <c r="F21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>119.99</v>
+      </c>
+      <c r="E22">
+        <f>C22*D22</f>
+        <v>239.98</v>
+      </c>
+      <c r="F22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>21.99</v>
+      </c>
+      <c r="E23">
+        <f>C23*D23</f>
+        <v>43.98</v>
+      </c>
+      <c r="F23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>22.95</v>
+      </c>
+      <c r="E24">
+        <f>C24*D24</f>
+        <v>45.9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>20.48</v>
+      </c>
+      <c r="E25">
+        <f>C25*D25</f>
+        <v>40.96</v>
+      </c>
+      <c r="F25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="E26">
+        <f>C26*D26</f>
+        <v>33.979999999999997</v>
+      </c>
+      <c r="F26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>12.99</v>
+      </c>
+      <c r="E27">
+        <f>C27*D27</f>
+        <v>25.98</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>12.99</v>
+      </c>
+      <c r="E28">
+        <f>C28*D28</f>
+        <v>38.97</v>
+      </c>
+      <c r="F28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>12.99</v>
+      </c>
+      <c r="E29">
+        <f>C29*D29</f>
+        <v>38.97</v>
+      </c>
+      <c r="F29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>49.99</v>
+      </c>
+      <c r="E30">
+        <f>C30*D30</f>
+        <v>99.98</v>
+      </c>
+      <c r="F30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>12.99</v>
+      </c>
+      <c r="E31">
+        <f>C31*D31</f>
+        <v>25.98</v>
+      </c>
+      <c r="F31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="E32">
+        <f>C32*D32</f>
+        <v>33.979999999999997</v>
+      </c>
+      <c r="F32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>11.99</v>
+      </c>
+      <c r="E33">
+        <f>C33*D33</f>
+        <v>23.98</v>
+      </c>
+      <c r="F33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="E34">
+        <f>C34*D34</f>
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="F34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>16.98</v>
+      </c>
+      <c r="E35">
+        <f>C35*D35</f>
+        <v>33.96</v>
+      </c>
+      <c r="F35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>15.99</v>
+      </c>
+      <c r="E36">
+        <f>C36*D36</f>
+        <v>63.96</v>
+      </c>
+      <c r="F36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>1.78</v>
+      </c>
+      <c r="E37">
+        <f>C37*D37</f>
+        <v>8.9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38">
         <v>6</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D38">
+        <v>1.28</v>
+      </c>
+      <c r="E38">
+        <f>C38*D38</f>
+        <v>7.68</v>
+      </c>
+      <c r="F38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>14.99</v>
+      </c>
+      <c r="E39">
+        <f>C39*D39</f>
+        <v>29.98</v>
+      </c>
+      <c r="F39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>6.99</v>
+      </c>
+      <c r="E40">
+        <f>C40*D40</f>
+        <v>13.98</v>
+      </c>
+      <c r="F40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>7.99</v>
+      </c>
+      <c r="E41">
+        <f>C41*D41</f>
+        <v>15.98</v>
+      </c>
+      <c r="F41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
         <v>7</v>
       </c>
-      <c r="C22">
+      <c r="C48">
         <v>1</v>
       </c>
-      <c r="D22">
+      <c r="D48">
         <v>2200</v>
       </c>
-      <c r="E22">
+      <c r="E48">
         <f t="shared" si="0"/>
         <v>2200</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
         <v>46</v>
       </c>
-      <c r="C23">
+      <c r="C49">
         <v>1</v>
       </c>
-      <c r="D23">
+      <c r="D49">
         <v>1460</v>
       </c>
-      <c r="E23">
+      <c r="E49">
         <f t="shared" si="0"/>
         <v>1460</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F49" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
         <v>50</v>
       </c>
-      <c r="B26">
-        <f>SUM(D2:D17)</f>
+      <c r="B51">
+        <f>SUM(D3:D18)</f>
         <v>1926.87</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52">
+        <f>SUM(E21:E41)</f>
+        <v>972.82000000000016</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>48</v>
       </c>
-      <c r="B27">
-        <f>SUM(E2:E23)</f>
-        <v>6763.24</v>
+      <c r="B53">
+        <f>SUM(E3:E49)</f>
+        <v>7736.0599999999995</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F24" r:id="rId1" xr:uid="{C779AFD3-8252-410C-8943-A367E910B41F}"/>
+    <hyperlink ref="F21" r:id="rId2" display="https://factorydirecthobbies.com/products/preorder-walthers-cornerstone-933-3656-eagle-point-lighthouse-kit-8-1-8-x-3-x-8-7-8-20-3-x-7-5-x-22-8cm-ho?variant=39291075657791&amp;currency=USD&amp;utm_medium=product_sync&amp;utm_source=google&amp;utm_content=sag_organic&amp;utm_campaign=sag_organic&amp;utm_campaign=gs-2020-09-16&amp;utm_source=google&amp;utm_medium=smart_campaign&amp;gclid=EAIaIQobChMI2_Lt9Yne8QIVvGxvBB27rQC5EAQYAiABEgK43fD_BwE" xr:uid="{F6F00892-5D89-42D2-B5FB-BCDC4FCFF9E2}"/>
+    <hyperlink ref="F23" r:id="rId3" xr:uid="{F4E7C557-DE7B-4530-B702-E0AA042100B2}"/>
+    <hyperlink ref="F22" r:id="rId4" xr:uid="{C01FDEF1-E505-4C03-98FF-BE8D2F323584}"/>
+    <hyperlink ref="F25" r:id="rId5" xr:uid="{9A9EB695-B1BB-4D3A-9A4D-C74DE60F525D}"/>
+    <hyperlink ref="F29" r:id="rId6" xr:uid="{8825F131-1FEB-426E-8E5A-EA4CFC32A212}"/>
+    <hyperlink ref="F34" r:id="rId7" xr:uid="{45C9810A-2174-4448-84F1-4A83E782CB70}"/>
+    <hyperlink ref="F39" r:id="rId8" xr:uid="{44CB67BD-85B6-413A-ACB1-2ECDFC176C6E}"/>
+    <hyperlink ref="A1" r:id="rId9" display="https://barmillsmodels.com/product/fishing-shack-ho/" xr:uid="{228CF75F-C7B3-4C79-842C-8F72CC90B911}"/>
+    <hyperlink ref="F26" r:id="rId10" display="https://factorydirecthobbies.com/products/preorder-walthers-cornerstone-933-3656-eagle-point-lighthouse-kit-8-1-8-x-3-x-8-7-8-20-3-x-7-5-x-22-8cm-ho?variant=39291075657791&amp;currency=USD&amp;utm_medium=product_sync&amp;utm_source=google&amp;utm_content=sag_organic&amp;utm_campaign=sag_organic&amp;utm_campaign=gs-2020-09-16&amp;utm_source=google&amp;utm_medium=smart_campaign&amp;gclid=EAIaIQobChMI2_Lt9Yne8QIVvGxvBB27rQC5EAQYAiABEgK43fD_BwE" xr:uid="{6C8C67C8-CED0-4813-BBBE-508614754C24}"/>
+    <hyperlink ref="F31" r:id="rId11" display="https://factorydirecthobbies.com/products/preorder-walthers-cornerstone-933-3656-eagle-point-lighthouse-kit-8-1-8-x-3-x-8-7-8-20-3-x-7-5-x-22-8cm-ho?variant=39291075657791&amp;currency=USD&amp;utm_medium=product_sync&amp;utm_source=google&amp;utm_content=sag_organic&amp;utm_campaign=sag_organic&amp;utm_campaign=gs-2020-09-16&amp;utm_source=google&amp;utm_medium=smart_campaign&amp;gclid=EAIaIQobChMI2_Lt9Yne8QIVvGxvBB27rQC5EAQYAiABEgK43fD_BwE" xr:uid="{91A66138-177E-498E-AB98-29181B6A765D}"/>
+    <hyperlink ref="F36" r:id="rId12" display="https://factorydirecthobbies.com/products/preorder-walthers-cornerstone-933-3656-eagle-point-lighthouse-kit-8-1-8-x-3-x-8-7-8-20-3-x-7-5-x-22-8cm-ho?variant=39291075657791&amp;currency=USD&amp;utm_medium=product_sync&amp;utm_source=google&amp;utm_content=sag_organic&amp;utm_campaign=sag_organic&amp;utm_campaign=gs-2020-09-16&amp;utm_source=google&amp;utm_medium=smart_campaign&amp;gclid=EAIaIQobChMI2_Lt9Yne8QIVvGxvBB27rQC5EAQYAiABEgK43fD_BwE" xr:uid="{E4A84A4E-2841-4EDE-BBC5-18B407CE251E}"/>
+    <hyperlink ref="F41" r:id="rId13" display="https://www.mapleleaftrains.com/catalog/76231-garden-shed/" xr:uid="{D428B05A-CA5D-44BA-9C50-44A3928853AB}"/>
+    <hyperlink ref="F28" r:id="rId14" xr:uid="{AEA93639-A393-4771-BA18-95C6583CD8E1}"/>
+    <hyperlink ref="F33" r:id="rId15" xr:uid="{CEBA83D9-1FC5-4E23-B7B6-D71568FFA230}"/>
+    <hyperlink ref="F38" r:id="rId16" xr:uid="{BE73F516-1EB6-4192-B58F-4BECEF3E996C}"/>
+    <hyperlink ref="F27" r:id="rId17" xr:uid="{45B0E4CA-3F39-4DC4-A2CB-14E6071BDAD2}"/>
+    <hyperlink ref="F32" r:id="rId18" xr:uid="{90912986-597E-46FA-A12E-2C67433FC24B}"/>
+    <hyperlink ref="F37" r:id="rId19" xr:uid="{A17F1985-2232-4E67-B2E1-3E7D06F58581}"/>
+    <hyperlink ref="F30" r:id="rId20" xr:uid="{8EC99989-86A0-4317-997E-F8C8C63C03A6}"/>
+    <hyperlink ref="F35" r:id="rId21" xr:uid="{7103B403-9215-43B3-9C32-EE2733B6464D}"/>
+    <hyperlink ref="F40" r:id="rId22" xr:uid="{937D68D6-7EDA-4CFF-8890-780D9C91563A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>